<commit_message>
more dummy data changes
</commit_message>
<xml_diff>
--- a/DataSets/TradeBlotterFX.xlsx
+++ b/DataSets/TradeBlotterFX.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdaptableTools/Code/adaptableblotter-demo/DataSets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="FXTrade" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -562,7 +567,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -572,11 +577,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J66" sqref="J66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="25.33203125" style="3" bestFit="1" customWidth="1"/>
@@ -593,7 +598,7 @@
     <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,7 +642,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -645,7 +650,7 @@
         <v>42332</v>
       </c>
       <c r="C2" s="3">
-        <f t="shared" ref="C2:C33" si="0">SUM(B2+1)</f>
+        <f>SUM(B2+1)</f>
         <v>42333</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -661,7 +666,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="5">
-        <f t="shared" ref="H2:H33" si="1">SUM(F2*I2*-1)</f>
+        <f>SUM(F2*I2*-1)</f>
         <v>56520000</v>
       </c>
       <c r="I2">
@@ -683,7 +688,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -691,7 +696,7 @@
         <v>42118</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B3+1)</f>
         <v>42119</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -707,7 +712,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F3*I3*-1)</f>
         <v>-1435200</v>
       </c>
       <c r="I3">
@@ -729,7 +734,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -737,7 +742,7 @@
         <v>42515</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B4+1)</f>
         <v>42516</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -753,7 +758,7 @@
         <v>6</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F4*I4*-1)</f>
         <v>-14352</v>
       </c>
       <c r="I4">
@@ -775,7 +780,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -783,7 +788,7 @@
         <v>42358</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B5+1)</f>
         <v>42359</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -799,7 +804,7 @@
         <v>55</v>
       </c>
       <c r="H5" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F5*I5*-1)</f>
         <v>1239075</v>
       </c>
       <c r="I5">
@@ -821,7 +826,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -829,7 +834,7 @@
         <v>42450</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B6+1)</f>
         <v>42451</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -845,7 +850,7 @@
         <v>41</v>
       </c>
       <c r="H6" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F6*I6*-1)</f>
         <v>39380000</v>
       </c>
       <c r="I6">
@@ -867,7 +872,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -875,7 +880,7 @@
         <v>42289</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B7+1)</f>
         <v>42290</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -891,7 +896,7 @@
         <v>6</v>
       </c>
       <c r="H7" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F7*I7*-1)</f>
         <v>-56520000</v>
       </c>
       <c r="I7">
@@ -913,7 +918,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -921,7 +926,7 @@
         <v>42157</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B8+1)</f>
         <v>42158</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -937,7 +942,7 @@
         <v>6</v>
       </c>
       <c r="H8" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F8*I8*-1)</f>
         <v>-717600</v>
       </c>
       <c r="I8">
@@ -959,7 +964,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -967,7 +972,7 @@
         <v>42283</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B9+1)</f>
         <v>42284</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -983,7 +988,7 @@
         <v>6</v>
       </c>
       <c r="H9" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F9*I9*-1)</f>
         <v>-565200</v>
       </c>
       <c r="I9">
@@ -1005,7 +1010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1013,7 +1018,7 @@
         <v>42187</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B10+1)</f>
         <v>42188</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1029,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="H10" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F10*I10*-1)</f>
         <v>-1130400</v>
       </c>
       <c r="I10">
@@ -1051,7 +1056,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1059,7 +1064,7 @@
         <v>42432</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B11+1)</f>
         <v>42433</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1075,7 +1080,7 @@
         <v>41</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F11*I11*-1)</f>
         <v>787600</v>
       </c>
       <c r="I11">
@@ -1097,7 +1102,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1105,7 +1110,7 @@
         <v>42479</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B12+1)</f>
         <v>42480</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1121,7 +1126,7 @@
         <v>41</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F12*I12*-1)</f>
         <v>7876</v>
       </c>
       <c r="I12">
@@ -1143,7 +1148,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1151,7 +1156,7 @@
         <v>42212</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B13+1)</f>
         <v>42213</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1167,7 +1172,7 @@
         <v>6</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F13*I13*-1)</f>
         <v>-11304</v>
       </c>
       <c r="I13">
@@ -1189,7 +1194,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1197,7 +1202,7 @@
         <v>42239</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B14+1)</f>
         <v>42240</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1213,7 +1218,7 @@
         <v>6</v>
       </c>
       <c r="H14" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F14*I14*-1)</f>
         <v>-565200</v>
       </c>
       <c r="I14">
@@ -1235,7 +1240,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1243,7 +1248,7 @@
         <v>42481</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B15+1)</f>
         <v>42482</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1259,7 +1264,7 @@
         <v>41</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F15*I15*-1)</f>
         <v>393800</v>
       </c>
       <c r="I15">
@@ -1281,7 +1286,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1289,7 +1294,7 @@
         <v>42082</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B16+1)</f>
         <v>42083</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1305,7 +1310,7 @@
         <v>6</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F16*I16*-1)</f>
         <v>-717600</v>
       </c>
       <c r="I16">
@@ -1327,7 +1332,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1335,7 +1340,7 @@
         <v>42482</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B17+1)</f>
         <v>42483</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1351,7 +1356,7 @@
         <v>41</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F17*I17*-1)</f>
         <v>787600</v>
       </c>
       <c r="I17">
@@ -1373,7 +1378,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1381,7 +1386,7 @@
         <v>42412</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B18+1)</f>
         <v>42413</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1397,7 +1402,7 @@
         <v>55</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F18*I18*-1)</f>
         <v>6195375000</v>
       </c>
       <c r="I18">
@@ -1419,7 +1424,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1427,7 +1432,7 @@
         <v>42459</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B19+1)</f>
         <v>42460</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1443,7 +1448,7 @@
         <v>41</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F19*I19*-1)</f>
         <v>7876</v>
       </c>
       <c r="I19">
@@ -1465,7 +1470,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1473,7 +1478,7 @@
         <v>42354</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B20+1)</f>
         <v>42355</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1489,7 +1494,7 @@
         <v>55</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F20*I20*-1)</f>
         <v>6195375000</v>
       </c>
       <c r="I20">
@@ -1511,7 +1516,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1519,7 +1524,7 @@
         <v>42097</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B21+1)</f>
         <v>42098</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -1535,7 +1540,7 @@
         <v>55</v>
       </c>
       <c r="H21" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F21*I21*-1)</f>
         <v>-5481125000</v>
       </c>
       <c r="I21">
@@ -1557,7 +1562,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1565,7 +1570,7 @@
         <v>42155</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B22+1)</f>
         <v>42156</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -1581,7 +1586,7 @@
         <v>55</v>
       </c>
       <c r="H22" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F22*I22*-1)</f>
         <v>-5481125000</v>
       </c>
       <c r="I22">
@@ -1603,7 +1608,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1611,7 +1616,7 @@
         <v>42122</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B23+1)</f>
         <v>42123</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -1627,7 +1632,7 @@
         <v>55</v>
       </c>
       <c r="H23" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F23*I23*-1)</f>
         <v>-1096225</v>
       </c>
       <c r="I23">
@@ -1649,7 +1654,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1657,7 +1662,7 @@
         <v>42276</v>
       </c>
       <c r="C24" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B24+1)</f>
         <v>42277</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -1673,7 +1678,7 @@
         <v>6</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F24*I24*-1)</f>
         <v>-565200</v>
       </c>
       <c r="I24">
@@ -1695,7 +1700,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1703,7 +1708,7 @@
         <v>42350</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B25+1)</f>
         <v>42351</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -1719,7 +1724,7 @@
         <v>55</v>
       </c>
       <c r="H25" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F25*I25*-1)</f>
         <v>1239075</v>
       </c>
       <c r="I25">
@@ -1741,7 +1746,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1749,7 +1754,7 @@
         <v>42487</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B26+1)</f>
         <v>42488</v>
       </c>
       <c r="D26" s="3" t="s">
@@ -1765,7 +1770,7 @@
         <v>41</v>
       </c>
       <c r="H26" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F26*I26*-1)</f>
         <v>7876</v>
       </c>
       <c r="I26">
@@ -1787,7 +1792,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1795,7 +1800,7 @@
         <v>42444</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B27+1)</f>
         <v>42445</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -1811,7 +1816,7 @@
         <v>41</v>
       </c>
       <c r="H27" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F27*I27*-1)</f>
         <v>39380000</v>
       </c>
       <c r="I27">
@@ -1833,7 +1838,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1841,7 +1846,7 @@
         <v>42270</v>
       </c>
       <c r="C28" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B28+1)</f>
         <v>42271</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -1857,7 +1862,7 @@
         <v>6</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F28*I28*-1)</f>
         <v>-56520000</v>
       </c>
       <c r="I28">
@@ -1879,7 +1884,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1887,7 +1892,7 @@
         <v>42174</v>
       </c>
       <c r="C29" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B29+1)</f>
         <v>42175</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -1903,7 +1908,7 @@
         <v>6</v>
       </c>
       <c r="H29" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F29*I29*-1)</f>
         <v>-1130400</v>
       </c>
       <c r="I29">
@@ -1925,7 +1930,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1933,7 +1938,7 @@
         <v>42253</v>
       </c>
       <c r="C30" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B30+1)</f>
         <v>42254</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -1949,7 +1954,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F30*I30*-1)</f>
         <v>-11304</v>
       </c>
       <c r="I30">
@@ -1971,7 +1976,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1979,7 +1984,7 @@
         <v>42226</v>
       </c>
       <c r="C31" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B31+1)</f>
         <v>42227</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -1995,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="H31" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F31*I31*-1)</f>
         <v>-56520000</v>
       </c>
       <c r="I31">
@@ -2017,7 +2022,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2025,7 +2030,7 @@
         <v>42030</v>
       </c>
       <c r="C32" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B32+1)</f>
         <v>42031</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -2041,7 +2046,7 @@
         <v>6</v>
       </c>
       <c r="H32" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F32*I32*-1)</f>
         <v>-14352</v>
       </c>
       <c r="I32">
@@ -2063,7 +2068,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2071,7 +2076,7 @@
         <v>42443</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" si="0"/>
+        <f>SUM(B33+1)</f>
         <v>42444</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -2087,7 +2092,7 @@
         <v>41</v>
       </c>
       <c r="H33" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(F33*I33*-1)</f>
         <v>7876</v>
       </c>
       <c r="I33">
@@ -2109,7 +2114,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2117,7 +2122,7 @@
         <v>42056</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" ref="C34:C65" si="2">SUM(B34+1)</f>
+        <f>SUM(B34+1)</f>
         <v>42057</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -2133,7 +2138,7 @@
         <v>6</v>
       </c>
       <c r="H34" s="5">
-        <f t="shared" ref="H34:H65" si="3">SUM(F34*I34*-1)</f>
+        <f>SUM(F34*I34*-1)</f>
         <v>-71760000</v>
       </c>
       <c r="I34">
@@ -2155,7 +2160,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2163,7 +2168,7 @@
         <v>42344</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B35+1)</f>
         <v>42345</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -2179,7 +2184,7 @@
         <v>55</v>
       </c>
       <c r="H35" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F35*I35*-1)</f>
         <v>61953750</v>
       </c>
       <c r="I35">
@@ -2201,7 +2206,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2209,7 +2214,7 @@
         <v>42099</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B36+1)</f>
         <v>42100</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -2225,7 +2230,7 @@
         <v>55</v>
       </c>
       <c r="H36" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F36*I36*-1)</f>
         <v>-1096225</v>
       </c>
       <c r="I36">
@@ -2247,7 +2252,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2255,7 +2260,7 @@
         <v>42314</v>
       </c>
       <c r="C37" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B37+1)</f>
         <v>42315</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -2271,7 +2276,7 @@
         <v>6</v>
       </c>
       <c r="H37" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F37*I37*-1)</f>
         <v>-56520000</v>
       </c>
       <c r="I37">
@@ -2293,7 +2298,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2301,7 +2306,7 @@
         <v>42357</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B38+1)</f>
         <v>42358</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -2317,7 +2322,7 @@
         <v>55</v>
       </c>
       <c r="H38" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F38*I38*-1)</f>
         <v>6195375000</v>
       </c>
       <c r="I38">
@@ -2339,7 +2344,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2347,7 +2352,7 @@
         <v>42130</v>
       </c>
       <c r="C39" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B39+1)</f>
         <v>42131</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -2363,7 +2368,7 @@
         <v>55</v>
       </c>
       <c r="H39" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F39*I39*-1)</f>
         <v>-5481125000</v>
       </c>
       <c r="I39">
@@ -2385,7 +2390,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2393,7 +2398,7 @@
         <v>42199</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B40+1)</f>
         <v>42200</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -2409,7 +2414,7 @@
         <v>6</v>
       </c>
       <c r="H40" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F40*I40*-1)</f>
         <v>-1130400</v>
       </c>
       <c r="I40">
@@ -2431,7 +2436,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2439,7 +2444,7 @@
         <v>42058</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B41+1)</f>
         <v>42059</v>
       </c>
       <c r="D41" s="3" t="s">
@@ -2455,7 +2460,7 @@
         <v>6</v>
       </c>
       <c r="H41" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F41*I41*-1)</f>
         <v>-14352</v>
       </c>
       <c r="I41">
@@ -2477,7 +2482,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2485,7 +2490,7 @@
         <v>42397</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B42+1)</f>
         <v>42398</v>
       </c>
       <c r="D42" s="3" t="s">
@@ -2501,7 +2506,7 @@
         <v>55</v>
       </c>
       <c r="H42" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F42*I42*-1)</f>
         <v>6195375000</v>
       </c>
       <c r="I42">
@@ -2523,7 +2528,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2531,7 +2536,7 @@
         <v>42375</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B43+1)</f>
         <v>42376</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -2547,7 +2552,7 @@
         <v>55</v>
       </c>
       <c r="H43" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F43*I43*-1)</f>
         <v>123907500</v>
       </c>
       <c r="I43">
@@ -2569,7 +2574,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2577,7 +2582,7 @@
         <v>42085</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B44+1)</f>
         <v>42086</v>
       </c>
       <c r="D44" s="3" t="s">
@@ -2593,7 +2598,7 @@
         <v>55</v>
       </c>
       <c r="H44" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F44*I44*-1)</f>
         <v>-5481125000</v>
       </c>
       <c r="I44">
@@ -2615,7 +2620,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2623,7 +2628,7 @@
         <v>42321</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B45+1)</f>
         <v>42322</v>
       </c>
       <c r="D45" s="3" t="s">
@@ -2639,7 +2644,7 @@
         <v>6</v>
       </c>
       <c r="H45" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F45*I45*-1)</f>
         <v>-56520000</v>
       </c>
       <c r="I45">
@@ -2661,7 +2666,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2669,7 +2674,7 @@
         <v>42024</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B46+1)</f>
         <v>42025</v>
       </c>
       <c r="D46" s="3" t="s">
@@ -2685,7 +2690,7 @@
         <v>6</v>
       </c>
       <c r="H46" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F46*I46*-1)</f>
         <v>-1435200</v>
       </c>
       <c r="I46">
@@ -2707,7 +2712,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2715,7 +2720,7 @@
         <v>42151</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B47+1)</f>
         <v>42152</v>
       </c>
       <c r="D47" s="3" t="s">
@@ -2731,7 +2736,7 @@
         <v>55</v>
       </c>
       <c r="H47" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F47*I47*-1)</f>
         <v>-109622500</v>
       </c>
       <c r="I47">
@@ -2753,7 +2758,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2761,7 +2766,7 @@
         <v>42464</v>
       </c>
       <c r="C48" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B48+1)</f>
         <v>42465</v>
       </c>
       <c r="D48" s="3" t="s">
@@ -2777,7 +2782,7 @@
         <v>41</v>
       </c>
       <c r="H48" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F48*I48*-1)</f>
         <v>39380000</v>
       </c>
       <c r="I48">
@@ -2799,7 +2804,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2807,7 +2812,7 @@
         <v>42447</v>
       </c>
       <c r="C49" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B49+1)</f>
         <v>42448</v>
       </c>
       <c r="D49" s="3" t="s">
@@ -2823,7 +2828,7 @@
         <v>41</v>
       </c>
       <c r="H49" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F49*I49*-1)</f>
         <v>39380000</v>
       </c>
       <c r="I49">
@@ -2845,7 +2850,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2853,7 +2858,7 @@
         <v>42106</v>
       </c>
       <c r="C50" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B50+1)</f>
         <v>42107</v>
       </c>
       <c r="D50" s="3" t="s">
@@ -2869,7 +2874,7 @@
         <v>55</v>
       </c>
       <c r="H50" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F50*I50*-1)</f>
         <v>-1096225</v>
       </c>
       <c r="I50">
@@ -2891,7 +2896,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2899,7 +2904,7 @@
         <v>42124</v>
       </c>
       <c r="C51" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B51+1)</f>
         <v>42125</v>
       </c>
       <c r="D51" s="3" t="s">
@@ -2915,7 +2920,7 @@
         <v>55</v>
       </c>
       <c r="H51" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F51*I51*-1)</f>
         <v>-109622500</v>
       </c>
       <c r="I51">
@@ -2937,7 +2942,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2945,7 +2950,7 @@
         <v>42394</v>
       </c>
       <c r="C52" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B52+1)</f>
         <v>42395</v>
       </c>
       <c r="D52" s="3" t="s">
@@ -2961,7 +2966,7 @@
         <v>55</v>
       </c>
       <c r="H52" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F52*I52*-1)</f>
         <v>61953750</v>
       </c>
       <c r="I52">
@@ -2983,7 +2988,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2991,7 +2996,7 @@
         <v>42444</v>
       </c>
       <c r="C53" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B53+1)</f>
         <v>42445</v>
       </c>
       <c r="D53" s="3" t="s">
@@ -3007,7 +3012,7 @@
         <v>56</v>
       </c>
       <c r="H53" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F53*I53*-1)</f>
         <v>12635</v>
       </c>
       <c r="I53">
@@ -3029,7 +3034,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3037,7 +3042,7 @@
         <v>42321</v>
       </c>
       <c r="C54" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B54+1)</f>
         <v>42322</v>
       </c>
       <c r="D54" s="3" t="s">
@@ -3053,7 +3058,7 @@
         <v>6</v>
       </c>
       <c r="H54" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F54*I54*-1)</f>
         <v>-56520000</v>
       </c>
       <c r="I54">
@@ -3075,7 +3080,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3083,7 +3088,7 @@
         <v>42086</v>
       </c>
       <c r="C55" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B55+1)</f>
         <v>42087</v>
       </c>
       <c r="D55" s="3" t="s">
@@ -3099,7 +3104,7 @@
         <v>55</v>
       </c>
       <c r="H55" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F55*I55*-1)</f>
         <v>-54811250</v>
       </c>
       <c r="I55">
@@ -3121,7 +3126,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3129,7 +3134,7 @@
         <v>42275</v>
       </c>
       <c r="C56" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B56+1)</f>
         <v>42276</v>
       </c>
       <c r="D56" s="3" t="s">
@@ -3145,7 +3150,7 @@
         <v>6</v>
       </c>
       <c r="H56" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F56*I56*-1)</f>
         <v>-782000</v>
       </c>
       <c r="I56">
@@ -3167,7 +3172,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3175,7 +3180,7 @@
         <v>42211</v>
       </c>
       <c r="C57" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B57+1)</f>
         <v>42212</v>
       </c>
       <c r="D57" s="3" t="s">
@@ -3191,7 +3196,7 @@
         <v>6</v>
       </c>
       <c r="H57" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F57*I57*-1)</f>
         <v>-565200</v>
       </c>
       <c r="I57">
@@ -3213,7 +3218,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3221,7 +3226,7 @@
         <v>42344</v>
       </c>
       <c r="C58" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B58+1)</f>
         <v>42345</v>
       </c>
       <c r="D58" s="3" t="s">
@@ -3237,7 +3242,7 @@
         <v>55</v>
       </c>
       <c r="H58" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F58*I58*-1)</f>
         <v>123907500</v>
       </c>
       <c r="I58">
@@ -3259,7 +3264,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3267,7 +3272,7 @@
         <v>42300</v>
       </c>
       <c r="C59" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B59+1)</f>
         <v>42301</v>
       </c>
       <c r="D59" s="3" t="s">
@@ -3283,7 +3288,7 @@
         <v>6</v>
       </c>
       <c r="H59" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F59*I59*-1)</f>
         <v>-7820</v>
       </c>
       <c r="I59">
@@ -3305,7 +3310,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3313,7 +3318,7 @@
         <v>42371</v>
       </c>
       <c r="C60" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B60+1)</f>
         <v>42372</v>
       </c>
       <c r="D60" s="3" t="s">
@@ -3329,7 +3334,7 @@
         <v>55</v>
       </c>
       <c r="H60" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F60*I60*-1)</f>
         <v>123907500</v>
       </c>
       <c r="I60">
@@ -3351,7 +3356,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3359,7 +3364,7 @@
         <v>42005</v>
       </c>
       <c r="C61" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B61+1)</f>
         <v>42006</v>
       </c>
       <c r="D61" s="3" t="s">
@@ -3375,7 +3380,7 @@
         <v>6</v>
       </c>
       <c r="H61" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F61*I61*-1)</f>
         <v>-14352</v>
       </c>
       <c r="I61">
@@ -3397,7 +3402,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3405,7 +3410,7 @@
         <v>42019</v>
       </c>
       <c r="C62" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B62+1)</f>
         <v>42020</v>
       </c>
       <c r="D62" s="3" t="s">
@@ -3421,7 +3426,7 @@
         <v>6</v>
       </c>
       <c r="H62" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F62*I62*-1)</f>
         <v>-1435200</v>
       </c>
       <c r="I62">
@@ -3443,7 +3448,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3451,7 +3456,7 @@
         <v>42484</v>
       </c>
       <c r="C63" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B63+1)</f>
         <v>42485</v>
       </c>
       <c r="D63" s="3" t="s">
@@ -3467,7 +3472,7 @@
         <v>56</v>
       </c>
       <c r="H63" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F63*I63*-1)</f>
         <v>1263500</v>
       </c>
       <c r="I63">
@@ -3489,7 +3494,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3497,7 +3502,7 @@
         <v>42030</v>
       </c>
       <c r="C64" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B64+1)</f>
         <v>42031</v>
       </c>
       <c r="D64" s="3" t="s">
@@ -3513,7 +3518,7 @@
         <v>6</v>
       </c>
       <c r="H64" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F64*I64*-1)</f>
         <v>-1435200</v>
       </c>
       <c r="I64">
@@ -3535,7 +3540,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3543,7 +3548,7 @@
         <v>42463</v>
       </c>
       <c r="C65" s="3">
-        <f t="shared" si="2"/>
+        <f>SUM(B65+1)</f>
         <v>42464</v>
       </c>
       <c r="D65" s="3" t="s">
@@ -3559,7 +3564,7 @@
         <v>56</v>
       </c>
       <c r="H65" s="5">
-        <f t="shared" si="3"/>
+        <f>SUM(F65*I65*-1)</f>
         <v>631750</v>
       </c>
       <c r="I65">
@@ -3581,7 +3586,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3589,7 +3594,7 @@
         <v>42403</v>
       </c>
       <c r="C66" s="3">
-        <f t="shared" ref="C66:C97" si="4">SUM(B66+1)</f>
+        <f>SUM(B66+1)</f>
         <v>42404</v>
       </c>
       <c r="D66" s="3" t="s">
@@ -3605,7 +3610,7 @@
         <v>55</v>
       </c>
       <c r="H66" s="5">
-        <f t="shared" ref="H66:H97" si="5">SUM(F66*I66*-1)</f>
+        <f>SUM(F66*I66*-1)</f>
         <v>123907500</v>
       </c>
       <c r="I66">
@@ -3627,7 +3632,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3635,7 +3640,7 @@
         <v>42037</v>
       </c>
       <c r="C67" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B67+1)</f>
         <v>42038</v>
       </c>
       <c r="D67" s="3" t="s">
@@ -3651,7 +3656,7 @@
         <v>6</v>
       </c>
       <c r="H67" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F67*I67*-1)</f>
         <v>-717600</v>
       </c>
       <c r="I67">
@@ -3673,7 +3678,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3681,7 +3686,7 @@
         <v>42157</v>
       </c>
       <c r="C68" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B68+1)</f>
         <v>42158</v>
       </c>
       <c r="D68" s="3" t="s">
@@ -3697,7 +3702,7 @@
         <v>55</v>
       </c>
       <c r="H68" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F68*I68*-1)</f>
         <v>-109622500</v>
       </c>
       <c r="I68">
@@ -3719,7 +3724,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3727,7 +3732,7 @@
         <v>42396</v>
       </c>
       <c r="C69" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B69+1)</f>
         <v>42397</v>
       </c>
       <c r="D69" s="3" t="s">
@@ -3743,7 +3748,7 @@
         <v>41</v>
       </c>
       <c r="H69" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F69*I69*-1)</f>
         <v>393800</v>
       </c>
       <c r="I69">
@@ -3765,7 +3770,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3773,7 +3778,7 @@
         <v>42383</v>
       </c>
       <c r="C70" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B70+1)</f>
         <v>42384</v>
       </c>
       <c r="D70" s="3" t="s">
@@ -3789,7 +3794,7 @@
         <v>41</v>
       </c>
       <c r="H70" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F70*I70*-1)</f>
         <v>787600</v>
       </c>
       <c r="I70">
@@ -3811,7 +3816,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3819,7 +3824,7 @@
         <v>42270</v>
       </c>
       <c r="C71" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B71+1)</f>
         <v>42271</v>
       </c>
       <c r="D71" s="3" t="s">
@@ -3835,7 +3840,7 @@
         <v>6</v>
       </c>
       <c r="H71" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F71*I71*-1)</f>
         <v>-391000</v>
       </c>
       <c r="I71">
@@ -3857,7 +3862,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3865,7 +3870,7 @@
         <v>42126</v>
       </c>
       <c r="C72" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B72+1)</f>
         <v>42127</v>
       </c>
       <c r="D72" s="3" t="s">
@@ -3881,7 +3886,7 @@
         <v>55</v>
       </c>
       <c r="H72" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F72*I72*-1)</f>
         <v>-109622500</v>
       </c>
       <c r="I72">
@@ -3903,7 +3908,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3911,7 +3916,7 @@
         <v>42282</v>
       </c>
       <c r="C73" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B73+1)</f>
         <v>42283</v>
       </c>
       <c r="D73" s="3" t="s">
@@ -3927,7 +3932,7 @@
         <v>6</v>
       </c>
       <c r="H73" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F73*I73*-1)</f>
         <v>-7820</v>
       </c>
       <c r="I73">
@@ -3949,7 +3954,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3957,7 +3962,7 @@
         <v>42260</v>
       </c>
       <c r="C74" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B74+1)</f>
         <v>42261</v>
       </c>
       <c r="D74" s="3" t="s">
@@ -3973,7 +3978,7 @@
         <v>6</v>
       </c>
       <c r="H74" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F74*I74*-1)</f>
         <v>-782000</v>
       </c>
       <c r="I74">
@@ -3995,7 +4000,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4003,7 +4008,7 @@
         <v>42297</v>
       </c>
       <c r="C75" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B75+1)</f>
         <v>42298</v>
       </c>
       <c r="D75" s="3" t="s">
@@ -4019,7 +4024,7 @@
         <v>6</v>
       </c>
       <c r="H75" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F75*I75*-1)</f>
         <v>-782000</v>
       </c>
       <c r="I75">
@@ -4041,7 +4046,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4049,7 +4054,7 @@
         <v>42202</v>
       </c>
       <c r="C76" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B76+1)</f>
         <v>42203</v>
       </c>
       <c r="D76" s="3" t="s">
@@ -4065,7 +4070,7 @@
         <v>6</v>
       </c>
       <c r="H76" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F76*I76*-1)</f>
         <v>-1130400</v>
       </c>
       <c r="I76">
@@ -4087,7 +4092,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4095,7 +4100,7 @@
         <v>42282</v>
       </c>
       <c r="C77" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B77+1)</f>
         <v>42283</v>
       </c>
       <c r="D77" s="3" t="s">
@@ -4111,7 +4116,7 @@
         <v>6</v>
       </c>
       <c r="H77" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F77*I77*-1)</f>
         <v>-39100000</v>
       </c>
       <c r="I77">
@@ -4133,7 +4138,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4141,7 +4146,7 @@
         <v>42037</v>
       </c>
       <c r="C78" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B78+1)</f>
         <v>42038</v>
       </c>
       <c r="D78" s="3" t="s">
@@ -4157,7 +4162,7 @@
         <v>6</v>
       </c>
       <c r="H78" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F78*I78*-1)</f>
         <v>-717600</v>
       </c>
       <c r="I78">
@@ -4179,7 +4184,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4187,7 +4192,7 @@
         <v>42456</v>
       </c>
       <c r="C79" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B79+1)</f>
         <v>42457</v>
       </c>
       <c r="D79" s="3" t="s">
@@ -4203,7 +4208,7 @@
         <v>56</v>
       </c>
       <c r="H79" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F79*I79*-1)</f>
         <v>12635</v>
       </c>
       <c r="I79">
@@ -4225,7 +4230,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4233,7 +4238,7 @@
         <v>42327</v>
       </c>
       <c r="C80" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B80+1)</f>
         <v>42328</v>
       </c>
       <c r="D80" s="3" t="s">
@@ -4249,7 +4254,7 @@
         <v>6</v>
       </c>
       <c r="H80" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F80*I80*-1)</f>
         <v>39100000</v>
       </c>
       <c r="I80">
@@ -4271,7 +4276,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4279,7 +4284,7 @@
         <v>42337</v>
       </c>
       <c r="C81" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B81+1)</f>
         <v>42338</v>
       </c>
       <c r="D81" s="3" t="s">
@@ -4295,7 +4300,7 @@
         <v>41</v>
       </c>
       <c r="H81" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F81*I81*-1)</f>
         <v>7876</v>
       </c>
       <c r="I81">
@@ -4317,7 +4322,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4325,7 +4330,7 @@
         <v>42482</v>
       </c>
       <c r="C82" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B82+1)</f>
         <v>42483</v>
       </c>
       <c r="D82" s="3" t="s">
@@ -4341,7 +4346,7 @@
         <v>56</v>
       </c>
       <c r="H82" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F82*I82*-1)</f>
         <v>75000000</v>
       </c>
       <c r="I82">
@@ -4363,7 +4368,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4371,7 +4376,7 @@
         <v>42325</v>
       </c>
       <c r="C83" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B83+1)</f>
         <v>42326</v>
       </c>
       <c r="D83" s="3" t="s">
@@ -4387,7 +4392,7 @@
         <v>6</v>
       </c>
       <c r="H83" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F83*I83*-1)</f>
         <v>-782000</v>
       </c>
       <c r="I83">
@@ -4409,7 +4414,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4417,7 +4422,7 @@
         <v>42068</v>
       </c>
       <c r="C84" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B84+1)</f>
         <v>42069</v>
       </c>
       <c r="D84" s="3" t="s">
@@ -4433,7 +4438,7 @@
         <v>6</v>
       </c>
       <c r="H84" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F84*I84*-1)</f>
         <v>-14352</v>
       </c>
       <c r="I84">
@@ -4455,7 +4460,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4463,7 +4468,7 @@
         <v>42130</v>
       </c>
       <c r="C85" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B85+1)</f>
         <v>42131</v>
       </c>
       <c r="D85" s="3" t="s">
@@ -4479,7 +4484,7 @@
         <v>55</v>
       </c>
       <c r="H85" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F85*I85*-1)</f>
         <v>-109622500</v>
       </c>
       <c r="I85">
@@ -4501,7 +4506,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4509,7 +4514,7 @@
         <v>42334</v>
       </c>
       <c r="C86" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B86+1)</f>
         <v>42335</v>
       </c>
       <c r="D86" s="3" t="s">
@@ -4525,7 +4530,7 @@
         <v>6</v>
       </c>
       <c r="H86" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F86*I86*-1)</f>
         <v>717600</v>
       </c>
       <c r="I86">
@@ -4547,7 +4552,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4555,7 +4560,7 @@
         <v>42088</v>
       </c>
       <c r="C87" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B87+1)</f>
         <v>42089</v>
       </c>
       <c r="D87" s="3" t="s">
@@ -4571,7 +4576,7 @@
         <v>55</v>
       </c>
       <c r="H87" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F87*I87*-1)</f>
         <v>-1239075</v>
       </c>
       <c r="I87">
@@ -4593,7 +4598,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4601,7 +4606,7 @@
         <v>42122</v>
       </c>
       <c r="C88" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B88+1)</f>
         <v>42123</v>
       </c>
       <c r="D88" s="3" t="s">
@@ -4617,7 +4622,7 @@
         <v>55</v>
       </c>
       <c r="H88" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F88*I88*-1)</f>
         <v>-1239075</v>
       </c>
       <c r="I88">
@@ -4639,7 +4644,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4647,7 +4652,7 @@
         <v>42472</v>
       </c>
       <c r="C89" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B89+1)</f>
         <v>42473</v>
       </c>
       <c r="D89" s="3" t="s">
@@ -4663,7 +4668,7 @@
         <v>43</v>
       </c>
       <c r="H89" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F89*I89*-1)</f>
         <v>970300</v>
       </c>
       <c r="I89">
@@ -4685,7 +4690,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4693,7 +4698,7 @@
         <v>42069</v>
       </c>
       <c r="C90" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B90+1)</f>
         <v>42070</v>
       </c>
       <c r="D90" s="3" t="s">
@@ -4709,7 +4714,7 @@
         <v>6</v>
       </c>
       <c r="H90" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F90*I90*-1)</f>
         <v>-71760000</v>
       </c>
       <c r="I90">
@@ -4731,7 +4736,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4739,7 +4744,7 @@
         <v>42390</v>
       </c>
       <c r="C91" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B91+1)</f>
         <v>42391</v>
       </c>
       <c r="D91" s="3" t="s">
@@ -4755,7 +4760,7 @@
         <v>41</v>
       </c>
       <c r="H91" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F91*I91*-1)</f>
         <v>39380000</v>
       </c>
       <c r="I91">
@@ -4777,7 +4782,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4785,7 +4790,7 @@
         <v>42472</v>
       </c>
       <c r="C92" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B92+1)</f>
         <v>42473</v>
       </c>
       <c r="D92" s="3" t="s">
@@ -4801,7 +4806,7 @@
         <v>43</v>
       </c>
       <c r="H92" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F92*I92*-1)</f>
         <v>9703</v>
       </c>
       <c r="I92">
@@ -4823,7 +4828,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4831,7 +4836,7 @@
         <v>42058</v>
       </c>
       <c r="C93" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B93+1)</f>
         <v>42059</v>
       </c>
       <c r="D93" s="3" t="s">
@@ -4847,7 +4852,7 @@
         <v>6</v>
       </c>
       <c r="H93" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F93*I93*-1)</f>
         <v>-1435200</v>
       </c>
       <c r="I93">
@@ -4869,7 +4874,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4877,7 +4882,7 @@
         <v>42261</v>
       </c>
       <c r="C94" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B94+1)</f>
         <v>42262</v>
       </c>
       <c r="D94" s="3" t="s">
@@ -4893,7 +4898,7 @@
         <v>6</v>
       </c>
       <c r="H94" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F94*I94*-1)</f>
         <v>-1435200</v>
       </c>
       <c r="I94">
@@ -4915,7 +4920,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4923,7 +4928,7 @@
         <v>42195</v>
       </c>
       <c r="C95" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B95+1)</f>
         <v>42196</v>
       </c>
       <c r="D95" s="3" t="s">
@@ -4939,7 +4944,7 @@
         <v>6</v>
       </c>
       <c r="H95" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F95*I95*-1)</f>
         <v>-565200</v>
       </c>
       <c r="I95">
@@ -4961,7 +4966,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4969,7 +4974,7 @@
         <v>42039</v>
       </c>
       <c r="C96" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B96+1)</f>
         <v>42040</v>
       </c>
       <c r="D96" s="3" t="s">
@@ -4985,7 +4990,7 @@
         <v>6</v>
       </c>
       <c r="H96" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F96*I96*-1)</f>
         <v>-14352</v>
       </c>
       <c r="I96">
@@ -5007,7 +5012,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="97" spans="1:14">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5015,7 +5020,7 @@
         <v>42414</v>
       </c>
       <c r="C97" s="3">
-        <f t="shared" si="4"/>
+        <f>SUM(B97+1)</f>
         <v>42415</v>
       </c>
       <c r="D97" s="3" t="s">
@@ -5031,7 +5036,7 @@
         <v>41</v>
       </c>
       <c r="H97" s="5">
-        <f t="shared" si="5"/>
+        <f>SUM(F97*I97*-1)</f>
         <v>787600</v>
       </c>
       <c r="I97">
@@ -5053,7 +5058,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5061,7 +5066,7 @@
         <v>42345</v>
       </c>
       <c r="C98" s="3">
-        <f t="shared" ref="C98:C129" si="6">SUM(B98+1)</f>
+        <f>SUM(B98+1)</f>
         <v>42346</v>
       </c>
       <c r="D98" s="3" t="s">
@@ -5077,7 +5082,7 @@
         <v>41</v>
       </c>
       <c r="H98" s="5">
-        <f t="shared" ref="H98:H129" si="7">SUM(F98*I98*-1)</f>
+        <f>SUM(F98*I98*-1)</f>
         <v>787600</v>
       </c>
       <c r="I98">
@@ -5099,7 +5104,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5107,7 +5112,7 @@
         <v>42124</v>
       </c>
       <c r="C99" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B99+1)</f>
         <v>42125</v>
       </c>
       <c r="D99" s="3" t="s">
@@ -5123,7 +5128,7 @@
         <v>55</v>
       </c>
       <c r="H99" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F99*I99*-1)</f>
         <v>-6195375000</v>
       </c>
       <c r="I99">
@@ -5145,7 +5150,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5153,7 +5158,7 @@
         <v>42420</v>
       </c>
       <c r="C100" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B100+1)</f>
         <v>42421</v>
       </c>
       <c r="D100" s="3" t="s">
@@ -5169,7 +5174,7 @@
         <v>43</v>
       </c>
       <c r="H100" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F100*I100*-1)</f>
         <v>48515000</v>
       </c>
       <c r="I100">
@@ -5191,7 +5196,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5199,7 +5204,7 @@
         <v>42489</v>
       </c>
       <c r="C101" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B101+1)</f>
         <v>42490</v>
       </c>
       <c r="D101" s="3" t="s">
@@ -5215,7 +5220,7 @@
         <v>43</v>
       </c>
       <c r="H101" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F101*I101*-1)</f>
         <v>48515000</v>
       </c>
       <c r="I101">
@@ -5237,7 +5242,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5245,7 +5250,7 @@
         <v>42504</v>
       </c>
       <c r="C102" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B102+1)</f>
         <v>42505</v>
       </c>
       <c r="D102" s="3" t="s">
@@ -5261,7 +5266,7 @@
         <v>6</v>
       </c>
       <c r="H102" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F102*I102*-1)</f>
         <v>56520000</v>
       </c>
       <c r="I102">
@@ -5283,7 +5288,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="103" spans="1:14">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5291,7 +5296,7 @@
         <v>42513</v>
       </c>
       <c r="C103" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B103+1)</f>
         <v>42514</v>
       </c>
       <c r="D103" s="3" t="s">
@@ -5307,7 +5312,7 @@
         <v>6</v>
       </c>
       <c r="H103" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F103*I103*-1)</f>
         <v>-1435200</v>
       </c>
       <c r="I103">
@@ -5329,7 +5334,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="104" spans="1:14">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5337,7 +5342,7 @@
         <v>42519</v>
       </c>
       <c r="C104" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B104+1)</f>
         <v>42520</v>
       </c>
       <c r="D104" s="3" t="s">
@@ -5353,7 +5358,7 @@
         <v>6</v>
       </c>
       <c r="H104" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F104*I104*-1)</f>
         <v>-14352</v>
       </c>
       <c r="I104">
@@ -5375,7 +5380,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5383,7 +5388,7 @@
         <v>42532</v>
       </c>
       <c r="C105" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B105+1)</f>
         <v>42533</v>
       </c>
       <c r="D105" s="3" t="s">
@@ -5399,7 +5404,7 @@
         <v>55</v>
       </c>
       <c r="H105" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F105*I105*-1)</f>
         <v>1239075</v>
       </c>
       <c r="I105">
@@ -5421,7 +5426,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5429,7 +5434,7 @@
         <v>42572</v>
       </c>
       <c r="C106" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B106+1)</f>
         <v>42573</v>
       </c>
       <c r="D106" s="3" t="s">
@@ -5445,7 +5450,7 @@
         <v>41</v>
       </c>
       <c r="H106" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F106*I106*-1)</f>
         <v>39380000</v>
       </c>
       <c r="I106">
@@ -5467,7 +5472,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5475,7 +5480,7 @@
         <v>42586</v>
       </c>
       <c r="C107" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B107+1)</f>
         <v>42587</v>
       </c>
       <c r="D107" s="3" t="s">
@@ -5491,7 +5496,7 @@
         <v>6</v>
       </c>
       <c r="H107" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F107*I107*-1)</f>
         <v>-56520000</v>
       </c>
       <c r="I107">
@@ -5513,7 +5518,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="108" spans="1:14">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5521,7 +5526,7 @@
         <v>42593</v>
       </c>
       <c r="C108" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B108+1)</f>
         <v>42594</v>
       </c>
       <c r="D108" s="3" t="s">
@@ -5537,7 +5542,7 @@
         <v>6</v>
       </c>
       <c r="H108" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F108*I108*-1)</f>
         <v>-717600</v>
       </c>
       <c r="I108">
@@ -5559,7 +5564,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="109" spans="1:14">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5567,7 +5572,7 @@
         <v>42634</v>
       </c>
       <c r="C109" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B109+1)</f>
         <v>42635</v>
       </c>
       <c r="D109" s="3" t="s">
@@ -5583,7 +5588,7 @@
         <v>6</v>
       </c>
       <c r="H109" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F109*I109*-1)</f>
         <v>-565200</v>
       </c>
       <c r="I109">
@@ -5605,7 +5610,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="110" spans="1:14">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5613,7 +5618,7 @@
         <v>42654</v>
       </c>
       <c r="C110" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B110+1)</f>
         <v>42655</v>
       </c>
       <c r="D110" s="3" t="s">
@@ -5629,7 +5634,7 @@
         <v>6</v>
       </c>
       <c r="H110" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F110*I110*-1)</f>
         <v>-1130400</v>
       </c>
       <c r="I110">
@@ -5651,7 +5656,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="111" spans="1:14">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5659,7 +5664,7 @@
         <v>42662</v>
       </c>
       <c r="C111" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B111+1)</f>
         <v>42663</v>
       </c>
       <c r="D111" s="3" t="s">
@@ -5675,7 +5680,7 @@
         <v>41</v>
       </c>
       <c r="H111" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F111*I111*-1)</f>
         <v>787600</v>
       </c>
       <c r="I111">
@@ -5697,7 +5702,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="112" spans="1:14">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5705,7 +5710,7 @@
         <v>42674</v>
       </c>
       <c r="C112" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B112+1)</f>
         <v>42675</v>
       </c>
       <c r="D112" s="3" t="s">
@@ -5721,7 +5726,7 @@
         <v>41</v>
       </c>
       <c r="H112" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F112*I112*-1)</f>
         <v>7876</v>
       </c>
       <c r="I112">
@@ -5743,7 +5748,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:14">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5751,7 +5756,7 @@
         <v>42679</v>
       </c>
       <c r="C113" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B113+1)</f>
         <v>42680</v>
       </c>
       <c r="D113" s="3" t="s">
@@ -5767,7 +5772,7 @@
         <v>6</v>
       </c>
       <c r="H113" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F113*I113*-1)</f>
         <v>-11304</v>
       </c>
       <c r="I113">
@@ -5789,7 +5794,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="1:14">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5797,7 +5802,7 @@
         <v>42688</v>
       </c>
       <c r="C114" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B114+1)</f>
         <v>42689</v>
       </c>
       <c r="D114" s="3" t="s">
@@ -5813,7 +5818,7 @@
         <v>6</v>
       </c>
       <c r="H114" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F114*I114*-1)</f>
         <v>-648100</v>
       </c>
       <c r="I114">
@@ -5835,7 +5840,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="115" spans="1:14">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5843,7 +5848,7 @@
         <v>42703</v>
       </c>
       <c r="C115" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B115+1)</f>
         <v>42704</v>
       </c>
       <c r="D115" s="3" t="s">
@@ -5859,7 +5864,7 @@
         <v>41</v>
       </c>
       <c r="H115" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F115*I115*-1)</f>
         <v>393800</v>
       </c>
       <c r="I115">
@@ -5881,7 +5886,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:14">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5889,7 +5894,7 @@
         <v>42708</v>
       </c>
       <c r="C116" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B116+1)</f>
         <v>42709</v>
       </c>
       <c r="D116" s="3" t="s">
@@ -5905,7 +5910,7 @@
         <v>6</v>
       </c>
       <c r="H116" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F116*I116*-1)</f>
         <v>-717600</v>
       </c>
       <c r="I116">
@@ -5927,7 +5932,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="117" spans="1:14">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5935,7 +5940,7 @@
         <v>42716</v>
       </c>
       <c r="C117" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B117+1)</f>
         <v>42717</v>
       </c>
       <c r="D117" s="3" t="s">
@@ -5951,7 +5956,7 @@
         <v>41</v>
       </c>
       <c r="H117" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F117*I117*-1)</f>
         <v>986500</v>
       </c>
       <c r="I117">
@@ -5973,7 +5978,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5981,7 +5986,7 @@
         <v>42723</v>
       </c>
       <c r="C118" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B118+1)</f>
         <v>42724</v>
       </c>
       <c r="D118" s="3" t="s">
@@ -5997,7 +6002,7 @@
         <v>55</v>
       </c>
       <c r="H118" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F118*I118*-1)</f>
         <v>6195375000</v>
       </c>
       <c r="I118">
@@ -6019,7 +6024,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="119" spans="1:14">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -6027,7 +6032,7 @@
         <v>42739</v>
       </c>
       <c r="C119" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B119+1)</f>
         <v>42740</v>
       </c>
       <c r="D119" s="3" t="s">
@@ -6043,7 +6048,7 @@
         <v>41</v>
       </c>
       <c r="H119" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F119*I119*-1)</f>
         <v>7876</v>
       </c>
       <c r="I119">
@@ -6065,7 +6070,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="120" spans="1:14">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -6073,7 +6078,7 @@
         <v>42754</v>
       </c>
       <c r="C120" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B120+1)</f>
         <v>42755</v>
       </c>
       <c r="D120" s="3" t="s">
@@ -6089,7 +6094,7 @@
         <v>55</v>
       </c>
       <c r="H120" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F120*I120*-1)</f>
         <v>6078445000</v>
       </c>
       <c r="I120">
@@ -6111,7 +6116,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -6119,7 +6124,7 @@
         <v>42777</v>
       </c>
       <c r="C121" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B121+1)</f>
         <v>42778</v>
       </c>
       <c r="D121" s="3" t="s">
@@ -6135,7 +6140,7 @@
         <v>55</v>
       </c>
       <c r="H121" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F121*I121*-1)</f>
         <v>-5481125000</v>
       </c>
       <c r="I121">
@@ -6157,7 +6162,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -6165,7 +6170,7 @@
         <v>42811</v>
       </c>
       <c r="C122" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B122+1)</f>
         <v>42812</v>
       </c>
       <c r="D122" s="3" t="s">
@@ -6181,7 +6186,7 @@
         <v>55</v>
       </c>
       <c r="H122" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F122*I122*-1)</f>
         <v>-5466280000</v>
       </c>
       <c r="I122">
@@ -6203,7 +6208,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -6211,7 +6216,7 @@
         <v>42844</v>
       </c>
       <c r="C123" s="3">
-        <f t="shared" si="6"/>
+        <f>SUM(B123+1)</f>
         <v>42845</v>
       </c>
       <c r="D123" s="3" t="s">
@@ -6227,7 +6232,7 @@
         <v>55</v>
       </c>
       <c r="H123" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(F123*I123*-1)</f>
         <v>-1076548</v>
       </c>
       <c r="I123">
@@ -6250,15 +6255,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:O123">
+  <sortState ref="A2:N123">
     <sortCondition ref="A2:A123"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>